<commit_message>
Additions to Business Plan
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
+++ b/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15140" yWindow="0" windowWidth="18100" windowHeight="15220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Buisness Projection" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -680,6 +680,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,7 +696,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -1033,8 +1035,8 @@
   </sheetPr>
   <dimension ref="A1:HA57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9:V13"/>
+    <sheetView showGridLines="0" topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1061,57 +1063,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:209" ht="59.25" customHeight="1">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
     </row>
     <row r="2" spans="1:209" ht="18">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
       <c r="G2" s="9"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="109" t="s">
+      <c r="J2" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="109"/>
-      <c r="T2" s="113" t="s">
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="113"/>
+      <c r="U2" s="114"/>
       <c r="V2" s="66"/>
       <c r="W2" s="66"/>
       <c r="X2" s="66"/>
@@ -2328,7 +2330,7 @@
         <f>Timesheets!M8</f>
         <v>1612.5</v>
       </c>
-      <c r="V10" s="114"/>
+      <c r="V10" s="109"/>
       <c r="W10" s="6" t="s">
         <v>49</v>
       </c>
@@ -2393,7 +2395,7 @@
         <f>Timesheets!M9</f>
         <v>1890.25</v>
       </c>
-      <c r="V11" s="114"/>
+      <c r="V11" s="109"/>
       <c r="W11" s="101" t="s">
         <v>50</v>
       </c>
@@ -2458,7 +2460,7 @@
         <f>Timesheets!M10</f>
         <v>1525</v>
       </c>
-      <c r="V12" s="114"/>
+      <c r="V12" s="109"/>
       <c r="W12" s="101" t="s">
         <v>51</v>
       </c>
@@ -2516,7 +2518,7 @@
         <f t="shared" si="0"/>
         <v>1141</v>
       </c>
-      <c r="U13" s="107">
+      <c r="U13" s="115">
         <f>Timesheets!M11</f>
         <v>0</v>
       </c>
@@ -2581,7 +2583,7 @@
         <f t="shared" si="0"/>
         <v>1232.75</v>
       </c>
-      <c r="U14" s="107">
+      <c r="U14" s="115">
         <f>Timesheets!M12</f>
         <v>0</v>
       </c>
@@ -2612,7 +2614,7 @@
       <c r="R15" s="77"/>
       <c r="S15" s="77"/>
       <c r="T15" s="107"/>
-      <c r="U15" s="107">
+      <c r="U15" s="115">
         <f>Timesheets!M13</f>
         <v>0</v>
       </c>
@@ -2858,7 +2860,7 @@
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U16" s="107">
+      <c r="U16" s="115">
         <f>Timesheets!M14</f>
         <v>0</v>
       </c>
@@ -2916,7 +2918,7 @@
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U17" s="107">
+      <c r="U17" s="115">
         <f>Timesheets!M15</f>
         <v>0</v>
       </c>
@@ -4233,11 +4235,11 @@
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="3"/>
-      <c r="J38" s="110" t="s">
+      <c r="J38" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="110"/>
-      <c r="L38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="112"/>
       <c r="M38" s="92"/>
       <c r="N38" s="94"/>
       <c r="O38" s="17" t="s">
@@ -4385,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33:R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4797,16 +4799,16 @@
       <c r="B11" s="80">
         <v>9</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="105"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="116"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="116"/>
       <c r="M11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4819,16 +4821,16 @@
       <c r="B12" s="81">
         <v>10</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
       <c r="M12" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4839,16 +4841,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="82"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="116"/>
+      <c r="L13" s="116"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:13">
@@ -4858,16 +4860,16 @@
       <c r="B14" s="80">
         <v>1</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="116"/>
       <c r="M14" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4880,16 +4882,16 @@
       <c r="B15" s="80">
         <v>2</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="116"/>
+      <c r="H15" s="116"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="116"/>
+      <c r="K15" s="116"/>
+      <c r="L15" s="116"/>
       <c r="M15" s="13">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
up to date time sheets and weekly reports
sorry I’m late again! changes to business plan are minimal and don’t
affect anything
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
+++ b/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
@@ -1037,8 +1037,8 @@
   </sheetPr>
   <dimension ref="A1:HA57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2616,10 +2616,7 @@
       <c r="R15" s="77"/>
       <c r="S15" s="77"/>
       <c r="T15" s="107"/>
-      <c r="U15" s="110">
-        <f>Timesheets!M13</f>
-        <v>0</v>
-      </c>
+      <c r="U15" s="110"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
@@ -3124,10 +3121,7 @@
       <c r="R21" s="77"/>
       <c r="S21" s="77"/>
       <c r="T21" s="107"/>
-      <c r="U21" s="107">
-        <f>Timesheets!M19</f>
-        <v>0</v>
-      </c>
+      <c r="U21" s="107"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>

</xml_diff>

<commit_message>
update financial report 3
business plan update of summer projections and total projections in
RED. financial report now contains management, utilities and financial
review sections.
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
+++ b/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="25600" windowHeight="16020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Buisness Projection" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>RENT DUE</t>
   </si>
@@ -92,6 +92,9 @@
     <t>TOTAL</t>
   </si>
   <si>
+    <t>PROJECTION=</t>
+  </si>
+  <si>
     <t>Week</t>
   </si>
   <si>
@@ -221,37 +224,10 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>Total Projection</t>
-  </si>
-  <si>
-    <t>Labour</t>
-  </si>
-  <si>
-    <t>Projection =</t>
-  </si>
-  <si>
     <t>Total Maximum Projection</t>
+  </si>
+  <si>
+    <t>Total Realistic Projection</t>
   </si>
 </sst>
 </file>
@@ -347,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,12 +404,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,7 +507,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -709,7 +679,6 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -725,7 +694,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,7 +709,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -1083,8 +1052,8 @@
   </sheetPr>
   <dimension ref="A1:HA57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E12" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1111,57 +1080,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:209" ht="59.25" customHeight="1">
-      <c r="A1" s="115" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
+      <c r="A1" s="113" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
     </row>
     <row r="2" spans="1:209" ht="18">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
       <c r="G2" s="9"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="112" t="s">
+      <c r="J2" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="116" t="s">
-        <v>63</v>
-      </c>
-      <c r="U2" s="116"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="114" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="114"/>
       <c r="V2" s="66"/>
       <c r="W2" s="66"/>
       <c r="X2" s="66"/>
@@ -1175,13 +1144,13 @@
     <row r="3" spans="1:209" s="1" customFormat="1">
       <c r="A3" s="16"/>
       <c r="B3" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="18">
         <v>632.70000000000005</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="18">
         <v>150</v>
@@ -1219,15 +1188,15 @@
         <v>16</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:209" s="14" customFormat="1">
       <c r="A4" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>0</v>
@@ -1243,7 +1212,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" s="72"/>
       <c r="K4" s="72"/>
@@ -1263,13 +1232,8 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
-      <c r="AB4" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC4" s="9">
-        <f>700+987.5+1243.75</f>
-        <v>2931.25</v>
-      </c>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="9"/>
@@ -1501,11 +1465,11 @@
       <c r="S5" s="75">
         <v>0</v>
       </c>
-      <c r="T5" s="107">
+      <c r="T5" s="106">
         <f>SUM(J5:S5)</f>
         <v>0</v>
       </c>
-      <c r="U5" s="107">
+      <c r="U5" s="106">
         <f>Timesheets!M3</f>
         <v>0</v>
       </c>
@@ -1515,13 +1479,8 @@
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="9"/>
-      <c r="AB5" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC5" s="106">
-        <f>SUM(U9:U12)</f>
-        <v>6327.75</v>
-      </c>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
       <c r="AD5" s="9"/>
       <c r="AE5" s="9"/>
       <c r="AF5" s="9"/>
@@ -1738,7 +1697,7 @@
       <c r="N6" s="75">
         <v>37.5</v>
       </c>
-      <c r="O6" s="103">
+      <c r="O6" s="102">
         <f>4*12.5</f>
         <v>50</v>
       </c>
@@ -1754,11 +1713,11 @@
       <c r="S6" s="75">
         <v>37.5</v>
       </c>
-      <c r="T6" s="107">
+      <c r="T6" s="106">
         <f t="shared" ref="T6:T31" si="0">SUM(J6:S6)</f>
         <v>700</v>
       </c>
-      <c r="U6" s="107">
+      <c r="U6" s="106">
         <f>Timesheets!M4</f>
         <v>700</v>
       </c>
@@ -1768,13 +1727,8 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
-      <c r="AB6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC6" s="106">
-        <f>SUM(U13:U18)</f>
-        <v>5762.25</v>
-      </c>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="9"/>
@@ -2006,29 +1960,24 @@
       <c r="S7" s="75">
         <v>62.5</v>
       </c>
-      <c r="T7" s="107">
+      <c r="T7" s="106">
         <f t="shared" si="0"/>
         <v>987.5</v>
       </c>
-      <c r="U7" s="107">
+      <c r="U7" s="106">
         <f>Timesheets!M5</f>
         <v>987.5</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
-      <c r="AB7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC7" s="106">
-        <f>SUM(U19:U23)</f>
-        <v>4681</v>
-      </c>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
       <c r="AD7" s="9"/>
       <c r="AE7" s="9"/>
       <c r="AF7" s="9"/>
@@ -2241,7 +2190,7 @@
       <c r="L8" s="77">
         <v>187.5</v>
       </c>
-      <c r="M8" s="104">
+      <c r="M8" s="103">
         <f>4*12.5</f>
         <v>50</v>
       </c>
@@ -2257,26 +2206,23 @@
       <c r="Q8" s="77">
         <v>125</v>
       </c>
-      <c r="R8" s="104">
+      <c r="R8" s="103">
         <f>4*12.5</f>
         <v>50</v>
       </c>
       <c r="S8" s="77">
         <v>131.25</v>
       </c>
-      <c r="T8" s="107">
+      <c r="T8" s="106">
         <f t="shared" si="0"/>
         <v>1243.75</v>
       </c>
-      <c r="U8" s="107">
+      <c r="U8" s="106">
         <f>Timesheets!M6</f>
         <v>1243.75</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:209" s="9" customFormat="1">
@@ -2308,40 +2254,37 @@
       <c r="L9" s="77">
         <v>187.5</v>
       </c>
-      <c r="M9" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="N9" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O9" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P9" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q9" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R9" s="105">
+      <c r="M9" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="N9" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O9" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="P9" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q9" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R9" s="104">
         <v>95.75</v>
       </c>
       <c r="S9" s="77">
         <v>187.5</v>
       </c>
-      <c r="T9" s="107">
+      <c r="T9" s="106">
         <f t="shared" si="0"/>
         <v>1324.5</v>
       </c>
-      <c r="U9" s="107">
+      <c r="U9" s="106">
         <f>Timesheets!M7</f>
         <v>1300</v>
       </c>
-      <c r="W9" s="101" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB9" s="9" t="s">
-        <v>70</v>
+      <c r="W9" s="100" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:209" s="10" customFormat="1">
@@ -2378,38 +2321,35 @@
       <c r="M10" s="77">
         <v>187.5</v>
       </c>
-      <c r="N10" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O10" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P10" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q10" s="105">
+      <c r="N10" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O10" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="P10" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q10" s="104">
         <v>95.75</v>
       </c>
       <c r="R10" s="77">
         <v>187.5</v>
       </c>
-      <c r="S10" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T10" s="107">
+      <c r="S10" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="T10" s="106">
         <f t="shared" si="0"/>
         <v>1416.25</v>
       </c>
-      <c r="U10" s="107">
+      <c r="U10" s="106">
         <f>Timesheets!M8</f>
         <v>1612.5</v>
       </c>
-      <c r="V10" s="109"/>
+      <c r="V10" s="108"/>
       <c r="W10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB10" s="101" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:209" s="6" customFormat="1">
@@ -2434,13 +2374,13 @@
       <c r="I11" s="76">
         <v>7</v>
       </c>
-      <c r="J11" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K11" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L11" s="105">
+      <c r="J11" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K11" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L11" s="104">
         <v>95.75</v>
       </c>
       <c r="M11" s="77">
@@ -2449,7 +2389,7 @@
       <c r="N11" s="77">
         <v>187.5</v>
       </c>
-      <c r="O11" s="105">
+      <c r="O11" s="104">
         <v>95.75</v>
       </c>
       <c r="P11" s="77">
@@ -2464,20 +2404,20 @@
       <c r="S11" s="77">
         <v>187.5</v>
       </c>
-      <c r="T11" s="107">
+      <c r="T11" s="106">
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
-      <c r="U11" s="107">
+      <c r="U11" s="106">
         <f>Timesheets!M9</f>
         <v>1890.25</v>
       </c>
-      <c r="V11" s="109"/>
-      <c r="W11" s="101" t="s">
-        <v>49</v>
+      <c r="V11" s="108"/>
+      <c r="W11" s="100" t="s">
+        <v>50</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:209" s="9" customFormat="1">
@@ -2508,38 +2448,38 @@
       <c r="L12" s="77">
         <v>187.5</v>
       </c>
-      <c r="M12" s="105">
+      <c r="M12" s="104">
         <v>95.75</v>
       </c>
       <c r="N12" s="77">
         <v>187.5</v>
       </c>
-      <c r="O12" s="105">
+      <c r="O12" s="104">
         <v>95.75</v>
       </c>
       <c r="P12" s="77">
         <v>187.5</v>
       </c>
-      <c r="Q12" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R12" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="S12" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T12" s="107">
+      <c r="Q12" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R12" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="S12" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="T12" s="106">
         <f t="shared" si="0"/>
         <v>1416.25</v>
       </c>
-      <c r="U12" s="107">
+      <c r="U12" s="106">
         <f>Timesheets!M10</f>
         <v>1525</v>
       </c>
-      <c r="V12" s="109"/>
-      <c r="W12" s="101" t="s">
-        <v>50</v>
+      <c r="V12" s="108"/>
+      <c r="W12" s="100" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:209" s="9" customFormat="1">
@@ -2561,46 +2501,46 @@
       <c r="I13" s="80">
         <v>9</v>
       </c>
-      <c r="J13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="M13" s="105">
+      <c r="J13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="M13" s="104">
         <v>95.75</v>
       </c>
       <c r="N13" s="77">
         <v>187.5</v>
       </c>
-      <c r="O13" s="105">
+      <c r="O13" s="104">
         <v>95.75</v>
       </c>
       <c r="P13" s="77">
         <v>187.5</v>
       </c>
-      <c r="Q13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="S13" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T13" s="107">
+      <c r="Q13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="S13" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="T13" s="106">
         <f t="shared" si="0"/>
         <v>1141</v>
       </c>
-      <c r="U13" s="110">
+      <c r="U13" s="109">
         <f>Timesheets!M11</f>
         <v>1637.5</v>
       </c>
-      <c r="W13" s="102" t="s">
-        <v>51</v>
+      <c r="W13" s="101" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:209" s="11" customFormat="1">
@@ -2626,28 +2566,28 @@
       <c r="I14" s="81">
         <v>10</v>
       </c>
-      <c r="J14" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K14" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L14" s="105">
+      <c r="J14" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K14" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L14" s="104">
         <v>95.75</v>
       </c>
       <c r="M14" s="77">
         <v>187.5</v>
       </c>
-      <c r="N14" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O14" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P14" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q14" s="105">
+      <c r="N14" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O14" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="P14" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q14" s="104">
         <v>95.75</v>
       </c>
       <c r="R14" s="77">
@@ -2656,11 +2596,11 @@
       <c r="S14" s="77">
         <v>187.5</v>
       </c>
-      <c r="T14" s="107">
+      <c r="T14" s="106">
         <f t="shared" si="0"/>
         <v>1232.75</v>
       </c>
-      <c r="U14" s="110">
+      <c r="U14" s="109">
         <f>Timesheets!M12</f>
         <v>1300</v>
       </c>
@@ -2668,7 +2608,7 @@
     </row>
     <row r="15" spans="1:209" s="14" customFormat="1">
       <c r="A15" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
@@ -2690,8 +2630,8 @@
       <c r="Q15" s="77"/>
       <c r="R15" s="77"/>
       <c r="S15" s="77"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="110"/>
+      <c r="T15" s="106"/>
+      <c r="U15" s="109"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
@@ -2900,41 +2840,41 @@
       <c r="I16" s="80">
         <v>1</v>
       </c>
-      <c r="J16" s="105">
-        <v>75</v>
-      </c>
-      <c r="K16" s="105">
-        <v>75</v>
-      </c>
-      <c r="L16" s="105">
-        <v>75</v>
-      </c>
-      <c r="M16" s="105">
-        <v>75</v>
-      </c>
-      <c r="N16" s="105">
-        <v>75</v>
-      </c>
-      <c r="O16" s="105">
-        <v>75</v>
-      </c>
-      <c r="P16" s="105">
-        <v>75</v>
-      </c>
-      <c r="Q16" s="105">
-        <v>75</v>
-      </c>
-      <c r="R16" s="105">
-        <v>75</v>
-      </c>
-      <c r="S16" s="105">
-        <v>75</v>
-      </c>
-      <c r="T16" s="107">
+      <c r="J16" s="104">
+        <v>75</v>
+      </c>
+      <c r="K16" s="104">
+        <v>75</v>
+      </c>
+      <c r="L16" s="104">
+        <v>75</v>
+      </c>
+      <c r="M16" s="104">
+        <v>75</v>
+      </c>
+      <c r="N16" s="104">
+        <v>75</v>
+      </c>
+      <c r="O16" s="104">
+        <v>75</v>
+      </c>
+      <c r="P16" s="104">
+        <v>75</v>
+      </c>
+      <c r="Q16" s="104">
+        <v>75</v>
+      </c>
+      <c r="R16" s="104">
+        <v>75</v>
+      </c>
+      <c r="S16" s="104">
+        <v>75</v>
+      </c>
+      <c r="T16" s="106">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U16" s="110">
+      <c r="U16" s="109">
         <f>Timesheets!M14</f>
         <v>993.5</v>
       </c>
@@ -2958,41 +2898,41 @@
       <c r="I17" s="80">
         <v>2</v>
       </c>
-      <c r="J17" s="105">
-        <v>75</v>
-      </c>
-      <c r="K17" s="105">
-        <v>75</v>
-      </c>
-      <c r="L17" s="105">
-        <v>75</v>
-      </c>
-      <c r="M17" s="105">
-        <v>75</v>
-      </c>
-      <c r="N17" s="105">
-        <v>75</v>
-      </c>
-      <c r="O17" s="105">
-        <v>75</v>
-      </c>
-      <c r="P17" s="105">
-        <v>75</v>
-      </c>
-      <c r="Q17" s="105">
-        <v>75</v>
-      </c>
-      <c r="R17" s="105">
-        <v>75</v>
-      </c>
-      <c r="S17" s="105">
-        <v>75</v>
-      </c>
-      <c r="T17" s="107">
+      <c r="J17" s="104">
+        <v>75</v>
+      </c>
+      <c r="K17" s="104">
+        <v>75</v>
+      </c>
+      <c r="L17" s="104">
+        <v>75</v>
+      </c>
+      <c r="M17" s="104">
+        <v>75</v>
+      </c>
+      <c r="N17" s="104">
+        <v>75</v>
+      </c>
+      <c r="O17" s="104">
+        <v>75</v>
+      </c>
+      <c r="P17" s="104">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="104">
+        <v>75</v>
+      </c>
+      <c r="R17" s="104">
+        <v>75</v>
+      </c>
+      <c r="S17" s="104">
+        <v>75</v>
+      </c>
+      <c r="T17" s="106">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U17" s="110">
+      <c r="U17" s="109">
         <f>Timesheets!M15</f>
         <v>818.75</v>
       </c>
@@ -3016,41 +2956,41 @@
       <c r="I18" s="80">
         <v>3</v>
       </c>
-      <c r="J18" s="105">
-        <v>75</v>
-      </c>
-      <c r="K18" s="105">
-        <v>75</v>
-      </c>
-      <c r="L18" s="105">
-        <v>75</v>
-      </c>
-      <c r="M18" s="105">
-        <v>75</v>
-      </c>
-      <c r="N18" s="105">
-        <v>75</v>
-      </c>
-      <c r="O18" s="105">
-        <v>75</v>
-      </c>
-      <c r="P18" s="105">
-        <v>75</v>
-      </c>
-      <c r="Q18" s="105">
-        <v>75</v>
-      </c>
-      <c r="R18" s="105">
-        <v>75</v>
-      </c>
-      <c r="S18" s="105">
-        <v>75</v>
-      </c>
-      <c r="T18" s="107">
+      <c r="J18" s="104">
+        <v>75</v>
+      </c>
+      <c r="K18" s="104">
+        <v>75</v>
+      </c>
+      <c r="L18" s="104">
+        <v>75</v>
+      </c>
+      <c r="M18" s="104">
+        <v>75</v>
+      </c>
+      <c r="N18" s="104">
+        <v>75</v>
+      </c>
+      <c r="O18" s="104">
+        <v>75</v>
+      </c>
+      <c r="P18" s="104">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="104">
+        <v>75</v>
+      </c>
+      <c r="R18" s="104">
+        <v>75</v>
+      </c>
+      <c r="S18" s="104">
+        <v>75</v>
+      </c>
+      <c r="T18" s="106">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U18" s="110">
+      <c r="U18" s="109">
         <f>Timesheets!M16</f>
         <v>1012.5</v>
       </c>
@@ -3074,41 +3014,41 @@
       <c r="I19" s="80">
         <v>4</v>
       </c>
-      <c r="J19" s="105">
-        <v>75</v>
-      </c>
-      <c r="K19" s="105">
-        <v>75</v>
-      </c>
-      <c r="L19" s="105">
-        <v>75</v>
-      </c>
-      <c r="M19" s="105">
-        <v>75</v>
-      </c>
-      <c r="N19" s="105">
-        <v>75</v>
-      </c>
-      <c r="O19" s="105">
-        <v>75</v>
-      </c>
-      <c r="P19" s="105">
-        <v>75</v>
-      </c>
-      <c r="Q19" s="105">
-        <v>75</v>
-      </c>
-      <c r="R19" s="105">
-        <v>75</v>
-      </c>
-      <c r="S19" s="105">
-        <v>75</v>
-      </c>
-      <c r="T19" s="107">
+      <c r="J19" s="104">
+        <v>75</v>
+      </c>
+      <c r="K19" s="104">
+        <v>75</v>
+      </c>
+      <c r="L19" s="104">
+        <v>75</v>
+      </c>
+      <c r="M19" s="104">
+        <v>75</v>
+      </c>
+      <c r="N19" s="104">
+        <v>75</v>
+      </c>
+      <c r="O19" s="104">
+        <v>75</v>
+      </c>
+      <c r="P19" s="104">
+        <v>75</v>
+      </c>
+      <c r="Q19" s="104">
+        <v>75</v>
+      </c>
+      <c r="R19" s="104">
+        <v>75</v>
+      </c>
+      <c r="S19" s="104">
+        <v>75</v>
+      </c>
+      <c r="T19" s="106">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U19" s="110">
+      <c r="U19" s="109">
         <f>Timesheets!M17</f>
         <v>887.5</v>
       </c>
@@ -3132,48 +3072,48 @@
       <c r="I20" s="80">
         <v>5</v>
       </c>
-      <c r="J20" s="105">
-        <v>75</v>
-      </c>
-      <c r="K20" s="105">
-        <v>75</v>
-      </c>
-      <c r="L20" s="105">
-        <v>75</v>
-      </c>
-      <c r="M20" s="105">
-        <v>75</v>
-      </c>
-      <c r="N20" s="105">
-        <v>75</v>
-      </c>
-      <c r="O20" s="105">
-        <v>75</v>
-      </c>
-      <c r="P20" s="105">
-        <v>75</v>
-      </c>
-      <c r="Q20" s="105">
-        <v>75</v>
-      </c>
-      <c r="R20" s="105">
-        <v>75</v>
-      </c>
-      <c r="S20" s="105">
-        <v>75</v>
-      </c>
-      <c r="T20" s="107">
+      <c r="J20" s="104">
+        <v>75</v>
+      </c>
+      <c r="K20" s="104">
+        <v>75</v>
+      </c>
+      <c r="L20" s="104">
+        <v>75</v>
+      </c>
+      <c r="M20" s="104">
+        <v>75</v>
+      </c>
+      <c r="N20" s="104">
+        <v>75</v>
+      </c>
+      <c r="O20" s="104">
+        <v>75</v>
+      </c>
+      <c r="P20" s="104">
+        <v>75</v>
+      </c>
+      <c r="Q20" s="104">
+        <v>75</v>
+      </c>
+      <c r="R20" s="104">
+        <v>75</v>
+      </c>
+      <c r="S20" s="104">
+        <v>75</v>
+      </c>
+      <c r="T20" s="106">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="U20" s="110">
+      <c r="U20" s="109">
         <f>Timesheets!M18</f>
         <v>1087.5</v>
       </c>
     </row>
     <row r="21" spans="1:209" s="14" customFormat="1">
       <c r="A21" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
@@ -3195,8 +3135,8 @@
       <c r="Q21" s="77"/>
       <c r="R21" s="77"/>
       <c r="S21" s="77"/>
-      <c r="T21" s="107"/>
-      <c r="U21" s="107"/>
+      <c r="T21" s="106"/>
+      <c r="U21" s="106"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
@@ -3405,41 +3345,41 @@
       <c r="I22" s="78">
         <v>1</v>
       </c>
-      <c r="J22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L22" s="105">
-        <v>95.75</v>
+      <c r="J22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="K22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="L22" s="77">
+        <v>187.5</v>
       </c>
       <c r="M22" s="77">
         <v>187.5</v>
       </c>
-      <c r="N22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q22" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R22" s="77">
-        <v>187.5</v>
+      <c r="N22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="O22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="P22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="Q22" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="R22" s="104">
+        <v>95.75</v>
       </c>
       <c r="S22" s="77">
         <v>187.5</v>
       </c>
-      <c r="T22" s="107">
-        <f>SUM(J22:S22)</f>
-        <v>1232.75</v>
-      </c>
-      <c r="U22" s="107">
+      <c r="T22" s="106">
+        <f t="shared" si="0"/>
+        <v>1783.25</v>
+      </c>
+      <c r="U22" s="106">
         <f>Timesheets!M20</f>
         <v>1125</v>
       </c>
@@ -3463,11 +3403,11 @@
       <c r="I23" s="78">
         <v>2</v>
       </c>
-      <c r="J23" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="K23" s="77">
-        <v>187.5</v>
+      <c r="J23" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K23" s="104">
+        <v>95.75</v>
       </c>
       <c r="L23" s="77">
         <v>187.5</v>
@@ -3478,7 +3418,7 @@
       <c r="N23" s="77">
         <v>187.5</v>
       </c>
-      <c r="O23" s="105">
+      <c r="O23" s="104">
         <v>95.75</v>
       </c>
       <c r="P23" s="77">
@@ -3493,16 +3433,16 @@
       <c r="S23" s="77">
         <v>187.5</v>
       </c>
-      <c r="T23" s="107">
+      <c r="T23" s="106">
         <f t="shared" si="0"/>
-        <v>1783.25</v>
-      </c>
-      <c r="U23" s="107">
+        <v>1599.75</v>
+      </c>
+      <c r="U23" s="106">
         <f>Timesheets!M21</f>
-        <v>1581</v>
+        <v>562.5</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:209" s="9" customFormat="1">
@@ -3524,14 +3464,14 @@
       <c r="I24" s="78">
         <v>3</v>
       </c>
-      <c r="J24" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="K24" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="L24" s="105">
-        <v>95.75</v>
+      <c r="J24" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K24" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L24" s="77">
+        <v>187.5</v>
       </c>
       <c r="M24" s="77">
         <v>187.5</v>
@@ -3539,8 +3479,8 @@
       <c r="N24" s="77">
         <v>187.5</v>
       </c>
-      <c r="O24" s="105">
-        <v>95.75</v>
+      <c r="O24" s="77">
+        <v>187.5</v>
       </c>
       <c r="P24" s="77">
         <v>187.5</v>
@@ -3554,11 +3494,11 @@
       <c r="S24" s="77">
         <v>187.5</v>
       </c>
-      <c r="T24" s="107">
+      <c r="T24" s="106">
         <f t="shared" si="0"/>
         <v>1691.5</v>
       </c>
-      <c r="U24" s="107">
+      <c r="U24" s="106">
         <f>Timesheets!M22</f>
         <v>0</v>
       </c>
@@ -3586,29 +3526,29 @@
       <c r="I25" s="76">
         <v>4</v>
       </c>
-      <c r="J25" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="K25" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="L25" s="105">
+      <c r="J25" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K25" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L25" s="104">
         <v>95.75</v>
       </c>
       <c r="M25" s="77">
         <v>187.5</v>
       </c>
-      <c r="N25" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="O25" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P25" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="Q25" s="77">
-        <v>187.5</v>
+      <c r="N25" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O25" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="P25" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q25" s="104">
+        <v>95.75</v>
       </c>
       <c r="R25" s="77">
         <v>187.5</v>
@@ -3616,11 +3556,11 @@
       <c r="S25" s="77">
         <v>187.5</v>
       </c>
-      <c r="T25" s="107">
+      <c r="T25" s="106">
         <f t="shared" si="0"/>
-        <v>1691.5</v>
-      </c>
-      <c r="U25" s="107">
+        <v>1232.75</v>
+      </c>
+      <c r="U25" s="106">
         <f>Timesheets!M23</f>
         <v>0</v>
       </c>
@@ -3645,28 +3585,28 @@
       <c r="I26" s="83">
         <v>5</v>
       </c>
-      <c r="J26" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K26" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L26" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="M26" s="77">
-        <v>187.5</v>
-      </c>
-      <c r="N26" s="105">
+      <c r="J26" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="K26" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="L26" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="M26" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="N26" s="104">
         <v>95.75</v>
       </c>
       <c r="O26" s="77">
         <v>187.5</v>
       </c>
-      <c r="P26" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q26" s="105">
+      <c r="P26" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q26" s="104">
         <v>95.75</v>
       </c>
       <c r="R26" s="77">
@@ -3675,16 +3615,16 @@
       <c r="S26" s="77">
         <v>187.5</v>
       </c>
-      <c r="T26" s="107">
+      <c r="T26" s="106">
         <f t="shared" si="0"/>
         <v>1416.25</v>
       </c>
-      <c r="U26" s="107">
+      <c r="U26" s="106">
         <f>Timesheets!M24</f>
         <v>0</v>
       </c>
-      <c r="W26" s="101" t="s">
-        <v>53</v>
+      <c r="W26" s="100" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:209" s="10" customFormat="1">
@@ -3709,23 +3649,23 @@
       <c r="I27" s="84">
         <v>6</v>
       </c>
-      <c r="J27" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K27" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L27" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="M27" s="105">
-        <v>95.75</v>
+      <c r="J27" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="K27" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="L27" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="M27" s="77">
+        <v>187.5</v>
       </c>
       <c r="N27" s="77">
         <v>187.5</v>
       </c>
-      <c r="O27" s="77">
-        <v>187.5</v>
+      <c r="O27" s="104">
+        <v>95.75</v>
       </c>
       <c r="P27" s="77">
         <v>187.5</v>
@@ -3733,17 +3673,17 @@
       <c r="Q27" s="77">
         <v>187.5</v>
       </c>
-      <c r="R27" s="105">
+      <c r="R27" s="104">
         <v>95.75</v>
       </c>
       <c r="S27" s="77">
         <v>187.5</v>
       </c>
-      <c r="T27" s="107">
+      <c r="T27" s="106">
         <f t="shared" si="0"/>
-        <v>1416.25</v>
-      </c>
-      <c r="U27" s="107">
+        <v>1691.5</v>
+      </c>
+      <c r="U27" s="106">
         <f>Timesheets!M25</f>
         <v>0</v>
       </c>
@@ -3771,46 +3711,46 @@
       <c r="I28" s="76">
         <v>7</v>
       </c>
-      <c r="J28" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K28" s="105">
-        <v>95.75</v>
+      <c r="J28" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="K28" s="77">
+        <v>187.5</v>
       </c>
       <c r="L28" s="77">
         <v>187.5</v>
       </c>
-      <c r="M28" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="N28" s="105">
+      <c r="M28" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="N28" s="104">
         <v>95.75</v>
       </c>
       <c r="O28" s="77">
         <v>187.5</v>
       </c>
-      <c r="P28" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q28" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R28" s="105">
-        <v>95.75</v>
+      <c r="P28" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q28" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R28" s="77">
+        <v>187.5</v>
       </c>
       <c r="S28" s="77">
         <v>187.5</v>
       </c>
-      <c r="T28" s="107">
+      <c r="T28" s="106">
         <f t="shared" si="0"/>
-        <v>1232.75</v>
-      </c>
-      <c r="U28" s="107">
+        <v>1599.75</v>
+      </c>
+      <c r="U28" s="106">
         <f>Timesheets!M26</f>
         <v>0</v>
       </c>
       <c r="W28" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:209" s="9" customFormat="1">
@@ -3838,16 +3778,16 @@
       <c r="K29" s="77">
         <v>187.5</v>
       </c>
-      <c r="L29" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="M29" s="105">
-        <v>95.75</v>
+      <c r="L29" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="M29" s="77">
+        <v>187.5</v>
       </c>
       <c r="N29" s="77">
         <v>187.5</v>
       </c>
-      <c r="O29" s="105">
+      <c r="O29" s="104">
         <v>95.75</v>
       </c>
       <c r="P29" s="77">
@@ -3859,14 +3799,14 @@
       <c r="R29" s="77">
         <v>187.5</v>
       </c>
-      <c r="S29" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T29" s="107">
+      <c r="S29" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="T29" s="106">
         <f t="shared" si="0"/>
-        <v>1508</v>
-      </c>
-      <c r="U29" s="107">
+        <v>1783.25</v>
+      </c>
+      <c r="U29" s="106">
         <f>Timesheets!M27</f>
         <v>0</v>
       </c>
@@ -3890,41 +3830,41 @@
       <c r="I30" s="83">
         <v>9</v>
       </c>
-      <c r="J30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="M30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="N30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="S30" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T30" s="107">
+      <c r="J30" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="K30" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="L30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="M30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="N30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O30" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="P30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="S30" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="T30" s="106">
         <f t="shared" si="0"/>
-        <v>957.5</v>
-      </c>
-      <c r="U30" s="107">
+        <v>1232.75</v>
+      </c>
+      <c r="U30" s="106">
         <f>Timesheets!M28</f>
         <v>0</v>
       </c>
@@ -3952,41 +3892,41 @@
       <c r="I31" s="81">
         <v>10</v>
       </c>
-      <c r="J31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="K31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="L31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="M31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="N31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="O31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="P31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="Q31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="R31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="S31" s="105">
-        <v>95.75</v>
-      </c>
-      <c r="T31" s="107">
+      <c r="J31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="K31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="L31" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="M31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="N31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="O31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="P31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="Q31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="R31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="S31" s="104">
+        <v>95.75</v>
+      </c>
+      <c r="T31" s="106">
         <f t="shared" si="0"/>
-        <v>957.5</v>
-      </c>
-      <c r="U31" s="107">
+        <v>1049.25</v>
+      </c>
+      <c r="U31" s="106">
         <f>Timesheets!M29</f>
         <v>0</v>
       </c>
@@ -4011,8 +3951,8 @@
       <c r="Q32" s="86"/>
       <c r="R32" s="86"/>
       <c r="S32" s="86"/>
-      <c r="T32" s="106"/>
-      <c r="U32" s="106"/>
+      <c r="T32" s="105"/>
+      <c r="U32" s="105"/>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
@@ -4111,14 +4051,14 @@
         <v>15817.500000000002</v>
       </c>
       <c r="C33" s="68" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D33" s="62">
         <f>SUM(D5:D31)</f>
         <v>3600</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F33" s="63">
         <f>B33+D33</f>
@@ -4131,27 +4071,27 @@
       <c r="I33" s="88"/>
       <c r="J33" s="89">
         <f t="shared" ref="J33:U33" si="1">SUM(J5:J31)</f>
-        <v>2936.75</v>
+        <v>3120.25</v>
       </c>
       <c r="K33" s="89">
         <f t="shared" si="1"/>
-        <v>2911.75</v>
+        <v>3095.25</v>
       </c>
       <c r="L33" s="89">
         <f t="shared" si="1"/>
-        <v>2845</v>
+        <v>3212</v>
       </c>
       <c r="M33" s="89">
-        <f>SUM(M5:M31)</f>
-        <v>2891</v>
+        <f t="shared" si="1"/>
+        <v>3074.5</v>
       </c>
       <c r="N33" s="89">
         <f t="shared" si="1"/>
         <v>2828.5</v>
       </c>
       <c r="O33" s="89">
-        <f t="shared" si="1"/>
-        <v>2432.25</v>
+        <f>SUM(O5:O31)</f>
+        <v>2615.75</v>
       </c>
       <c r="P33" s="89">
         <f t="shared" si="1"/>
@@ -4167,15 +4107,15 @@
       </c>
       <c r="S33" s="89">
         <f t="shared" si="1"/>
-        <v>3055.75</v>
+        <v>3147.5</v>
       </c>
       <c r="T33" s="89">
         <f t="shared" si="1"/>
-        <v>28607.25</v>
+        <v>29800</v>
       </c>
       <c r="U33" s="89">
         <f t="shared" si="1"/>
-        <v>19702.25</v>
+        <v>18683.75</v>
       </c>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
@@ -4271,9 +4211,6 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="8"/>
-      <c r="J34" s="117" t="s">
-        <v>73</v>
-      </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
@@ -4282,17 +4219,17 @@
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
       <c r="R34" s="95" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S34" s="96">
         <f>SUM(J33:S33)</f>
-        <v>28607.25</v>
+        <v>29800</v>
       </c>
       <c r="U34" s="9"/>
     </row>
     <row r="35" spans="1:109">
       <c r="J35" s="64" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="K35" s="65">
         <f>10*15*25*12.5</f>
@@ -4301,7 +4238,7 @@
     </row>
     <row r="36" spans="1:109">
       <c r="J36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:109">
@@ -4309,43 +4246,43 @@
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="3"/>
-      <c r="J38" s="113" t="s">
-        <v>37</v>
-      </c>
-      <c r="K38" s="113"/>
-      <c r="L38" s="114"/>
+      <c r="J38" s="111" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" s="111"/>
+      <c r="L38" s="112"/>
       <c r="M38" s="92"/>
       <c r="N38" s="94"/>
       <c r="O38" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P38" s="86"/>
       <c r="R38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:109">
       <c r="A39" s="3"/>
       <c r="J39" s="91" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K39" s="93"/>
       <c r="L39" s="93"/>
       <c r="M39" s="93"/>
       <c r="N39" s="93"/>
       <c r="O39" s="86" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P39" s="86"/>
     </row>
     <row r="40" spans="1:109">
-      <c r="J40" s="98" t="s">
-        <v>24</v>
+      <c r="J40" s="97" t="s">
+        <v>25</v>
       </c>
       <c r="K40" s="93"/>
       <c r="L40" s="93"/>
       <c r="M40" s="93"/>
-      <c r="N40" s="100"/>
+      <c r="N40" s="99"/>
       <c r="O40" s="90">
         <f>(20*24)+(40*3)</f>
         <v>600</v>
@@ -4354,42 +4291,42 @@
     </row>
     <row r="41" spans="1:109">
       <c r="J41" s="91" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K41" s="93"/>
       <c r="L41" s="93"/>
       <c r="M41" s="93"/>
-      <c r="N41" s="100"/>
+      <c r="N41" s="99"/>
       <c r="O41" s="90">
         <v>10000</v>
       </c>
       <c r="P41" s="86" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:109">
       <c r="J42" s="91" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K42" s="93"/>
       <c r="L42" s="93"/>
       <c r="M42" s="93"/>
-      <c r="N42" s="100"/>
+      <c r="N42" s="99"/>
       <c r="O42" s="90">
         <v>7000</v>
       </c>
       <c r="P42" s="86" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:109">
-      <c r="J43" s="99" t="s">
-        <v>38</v>
+      <c r="J43" s="98" t="s">
+        <v>39</v>
       </c>
       <c r="K43" s="93"/>
       <c r="L43" s="93"/>
       <c r="M43" s="93"/>
-      <c r="N43" s="100"/>
+      <c r="N43" s="99"/>
       <c r="O43" s="90">
         <f>O42*0.25</f>
         <v>1750</v>
@@ -4397,57 +4334,57 @@
       <c r="P43" s="86"/>
     </row>
     <row r="44" spans="1:109">
-      <c r="J44" s="99" t="s">
-        <v>39</v>
+      <c r="J44" s="98" t="s">
+        <v>40</v>
       </c>
       <c r="K44" s="93"/>
       <c r="L44" s="93"/>
       <c r="M44" s="93"/>
-      <c r="N44" s="100"/>
+      <c r="N44" s="99"/>
       <c r="O44" s="90">
         <f>O42*0.5</f>
         <v>3500</v>
       </c>
       <c r="P44" s="86"/>
-      <c r="R44" t="s">
-        <v>75</v>
+      <c r="R44" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:109">
-      <c r="J45" s="99" t="s">
-        <v>40</v>
+      <c r="J45" s="98" t="s">
+        <v>41</v>
       </c>
       <c r="K45" s="93"/>
       <c r="L45" s="93"/>
       <c r="M45" s="93"/>
-      <c r="N45" s="100"/>
+      <c r="N45" s="99"/>
       <c r="O45" s="90">
         <f>O42*0.25</f>
         <v>1750</v>
       </c>
       <c r="P45" s="86"/>
-      <c r="R45" s="97">
-        <f>F33+K35+O40</f>
+      <c r="R45" s="116">
+        <f>K35+O40+F33</f>
         <v>66892.5</v>
       </c>
     </row>
     <row r="46" spans="1:109">
-      <c r="R46" t="s">
-        <v>72</v>
+      <c r="R46" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:109">
       <c r="J47" t="s">
-        <v>28</v>
-      </c>
-      <c r="R47" s="97">
+        <v>29</v>
+      </c>
+      <c r="R47" s="116">
         <f>S34+O40+F33</f>
-        <v>48624.75</v>
+        <v>49817.5</v>
       </c>
     </row>
     <row r="48" spans="1:109">
       <c r="J48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="7:7">
@@ -4473,10 +4410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4519,7 +4456,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4527,7 +4464,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
@@ -4605,7 +4542,7 @@
       <c r="G4" s="75">
         <v>37.5</v>
       </c>
-      <c r="H4" s="103">
+      <c r="H4" s="102">
         <f>4*12.5</f>
         <v>50</v>
       </c>
@@ -4684,7 +4621,7 @@
       <c r="E6" s="77">
         <v>187.5</v>
       </c>
-      <c r="F6" s="104">
+      <c r="F6" s="103">
         <f>4*12.5</f>
         <v>50</v>
       </c>
@@ -4700,7 +4637,7 @@
       <c r="J6" s="77">
         <v>125</v>
       </c>
-      <c r="K6" s="104">
+      <c r="K6" s="103">
         <f>4*12.5</f>
         <v>50</v>
       </c>
@@ -4728,22 +4665,22 @@
       <c r="E7" s="77">
         <v>125</v>
       </c>
-      <c r="F7" s="105">
+      <c r="F7" s="104">
         <v>250</v>
       </c>
-      <c r="G7" s="105">
+      <c r="G7" s="104">
         <v>150</v>
       </c>
-      <c r="H7" s="105">
+      <c r="H7" s="104">
         <v>100</v>
       </c>
       <c r="I7" s="75">
         <v>125</v>
       </c>
-      <c r="J7" s="105">
+      <c r="J7" s="104">
         <v>62.5</v>
       </c>
-      <c r="K7" s="105">
+      <c r="K7" s="104">
         <v>125</v>
       </c>
       <c r="L7" s="77">
@@ -4773,22 +4710,22 @@
       <c r="F8" s="77">
         <v>100</v>
       </c>
-      <c r="G8" s="105">
+      <c r="G8" s="104">
         <v>125</v>
       </c>
-      <c r="H8" s="105">
+      <c r="H8" s="104">
         <v>175</v>
       </c>
       <c r="I8" s="75">
         <v>162.5</v>
       </c>
-      <c r="J8" s="105">
+      <c r="J8" s="104">
         <v>137.5</v>
       </c>
       <c r="K8" s="77">
         <v>137.5</v>
       </c>
-      <c r="L8" s="105">
+      <c r="L8" s="104">
         <v>262.5</v>
       </c>
       <c r="M8" s="13">
@@ -4803,13 +4740,13 @@
       <c r="B9" s="76">
         <v>7</v>
       </c>
-      <c r="C9" s="105">
+      <c r="C9" s="104">
         <v>237.5</v>
       </c>
-      <c r="D9" s="105">
+      <c r="D9" s="104">
         <v>150</v>
       </c>
-      <c r="E9" s="105">
+      <c r="E9" s="104">
         <v>150</v>
       </c>
       <c r="F9" s="77">
@@ -4818,7 +4755,7 @@
       <c r="G9" s="77">
         <v>112.5</v>
       </c>
-      <c r="H9" s="105">
+      <c r="H9" s="104">
         <v>137.5</v>
       </c>
       <c r="I9" s="75">
@@ -4854,13 +4791,13 @@
       <c r="E10" s="77">
         <v>150</v>
       </c>
-      <c r="F10" s="105">
+      <c r="F10" s="104">
         <v>175</v>
       </c>
       <c r="G10" s="77">
         <v>125</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H10" s="104">
         <v>150</v>
       </c>
       <c r="I10" s="75">
@@ -4869,10 +4806,10 @@
       <c r="J10" s="77">
         <v>62.5</v>
       </c>
-      <c r="K10" s="105">
-        <v>187.5</v>
-      </c>
-      <c r="L10" s="105">
+      <c r="K10" s="104">
+        <v>187.5</v>
+      </c>
+      <c r="L10" s="104">
         <v>312.5</v>
       </c>
       <c r="M10" s="13">
@@ -4978,7 +4915,7 @@
       <c r="I13" s="77"/>
       <c r="J13" s="77"/>
       <c r="K13" s="77" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L13" s="77"/>
       <c r="M13" s="13"/>
@@ -5238,10 +5175,10 @@
       <c r="I20" s="77">
         <v>187.5</v>
       </c>
-      <c r="J20" s="105">
+      <c r="J20" s="104">
         <v>62.5</v>
       </c>
-      <c r="K20" s="105">
+      <c r="K20" s="104">
         <v>187.5</v>
       </c>
       <c r="L20" s="77">
@@ -5259,40 +5196,27 @@
       <c r="B21" s="78">
         <v>2</v>
       </c>
-      <c r="C21" s="111">
-        <v>162.25</v>
-      </c>
-      <c r="D21" s="111">
-        <f>15*12.5</f>
-        <v>187.5</v>
-      </c>
-      <c r="E21" s="111">
-        <v>187.5</v>
-      </c>
-      <c r="F21" s="111">
-        <v>193.75</v>
-      </c>
-      <c r="G21" s="111">
-        <v>112.5</v>
-      </c>
-      <c r="H21" s="111">
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104">
         <v>50</v>
       </c>
-      <c r="I21" s="111">
+      <c r="I21" s="104">
         <v>175</v>
       </c>
-      <c r="J21" s="111">
+      <c r="J21" s="104">
         <v>162.5</v>
       </c>
-      <c r="K21" s="111">
+      <c r="K21" s="104">
         <v>175</v>
       </c>
-      <c r="L21" s="111">
-        <v>175</v>
-      </c>
+      <c r="L21" s="104"/>
       <c r="M21" s="13">
         <f t="shared" si="0"/>
-        <v>1581</v>
+        <v>562.5</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -5302,16 +5226,16 @@
       <c r="B22" s="78">
         <v>3</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
       <c r="G22" s="77"/>
-      <c r="H22" s="105"/>
+      <c r="H22" s="104"/>
       <c r="I22" s="77"/>
       <c r="J22" s="77"/>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
       <c r="M22" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5324,16 +5248,16 @@
       <c r="B23" s="76">
         <v>4</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="104"/>
       <c r="M23" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5346,16 +5270,16 @@
       <c r="B24" s="83">
         <v>5</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="105"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
       <c r="M24" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5368,16 +5292,16 @@
       <c r="B25" s="84">
         <v>6</v>
       </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="104"/>
       <c r="G25" s="77"/>
-      <c r="H25" s="105"/>
+      <c r="H25" s="104"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
-      <c r="K25" s="105"/>
-      <c r="L25" s="105"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="104"/>
       <c r="M25" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5390,16 +5314,16 @@
       <c r="B26" s="76">
         <v>7</v>
       </c>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="105"/>
-      <c r="L26" s="105"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="104"/>
       <c r="M26" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5414,14 +5338,14 @@
       </c>
       <c r="C27" s="77"/>
       <c r="D27" s="77"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
       <c r="G27" s="77"/>
-      <c r="H27" s="105"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
       <c r="K27" s="77"/>
-      <c r="L27" s="105"/>
+      <c r="L27" s="104"/>
       <c r="M27" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5434,16 +5358,16 @@
       <c r="B28" s="83">
         <v>9</v>
       </c>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
-      <c r="H28" s="105"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="105"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
       <c r="M28" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5456,16 +5380,16 @@
       <c r="B29" s="81">
         <v>10</v>
       </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="104"/>
+      <c r="L29" s="104"/>
       <c r="M29" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5473,27 +5397,27 @@
     </row>
     <row r="31" spans="1:13">
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="12">
         <f>SUM(C3:C29)</f>
-        <v>1999.75</v>
+        <v>1837.5</v>
       </c>
       <c r="D31" s="12">
         <f>SUM(D3:D29)</f>
-        <v>2362.5</v>
+        <v>2175</v>
       </c>
       <c r="E31" s="12">
         <f>SUM(E3:E29)</f>
-        <v>1712.5</v>
+        <v>1525</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" ref="F31:M31" si="1">SUM(F3:F29)</f>
-        <v>2708.75</v>
+        <v>2515</v>
       </c>
       <c r="G31" s="12">
         <f t="shared" si="1"/>
-        <v>1275</v>
+        <v>1162.5</v>
       </c>
       <c r="H31" s="12">
         <f t="shared" si="1"/>
@@ -5513,11 +5437,37 @@
       </c>
       <c r="L31" s="12">
         <f t="shared" si="1"/>
-        <v>2706.25</v>
-      </c>
-      <c r="M31" s="108">
+        <v>2531.25</v>
+      </c>
+      <c r="M31" s="107">
         <f t="shared" si="1"/>
-        <v>19702.25</v>
+        <v>18683.75</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13">
+      <c r="C37" s="12">
+        <f>SUM(C14:L18)</f>
+        <v>4799.75</v>
+      </c>
+      <c r="M37" s="12">
+        <f>SUM(M14:M18)</f>
+        <v>4799.75</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13">
+      <c r="C38" s="12">
+        <f>((C37/12.5)/10)/5</f>
+        <v>7.6796000000000006</v>
+      </c>
+      <c r="M38" s="115">
+        <f>SUM('Buisness Projection'!T16:T20)</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13">
+      <c r="M39" s="12">
+        <f>M37-M38</f>
+        <v>1049.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated time sheets on business plan
and added comments to random calculations on back page for readability.
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
+++ b/Documents/Finance/Financial Report 3 Submission/Business plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="17560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Buisness Projection" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam Beedell</author>
+  </authors>
+  <commentList>
+    <comment ref="I37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam Beedell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+overspend on labour for spring term
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam Beedell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+hours worked on average over easter
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam Beedell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+over spend on labour during  easter break</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
@@ -238,7 +322,7 @@
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +405,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -469,7 +566,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -506,8 +603,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -694,6 +793,8 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,10 +810,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="38">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -732,6 +832,7 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -748,6 +849,7 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1052,8 +1154,8 @@
   </sheetPr>
   <dimension ref="A1:HA57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L5" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView showGridLines="0" topLeftCell="N8" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1080,57 +1182,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:209" ht="59.25" customHeight="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
     </row>
     <row r="2" spans="1:209" ht="18">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
       <c r="G2" s="9"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="110" t="s">
+      <c r="J2" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="114" t="s">
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="114"/>
+      <c r="U2" s="116"/>
       <c r="V2" s="66"/>
       <c r="W2" s="66"/>
       <c r="X2" s="66"/>
@@ -3439,7 +3541,7 @@
       </c>
       <c r="U23" s="106">
         <f>Timesheets!M21</f>
-        <v>562.5</v>
+        <v>1581.25</v>
       </c>
       <c r="W23" s="9" t="s">
         <v>53</v>
@@ -4115,7 +4217,7 @@
       </c>
       <c r="U33" s="89">
         <f t="shared" si="1"/>
-        <v>18683.75</v>
+        <v>19702.5</v>
       </c>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
@@ -4246,11 +4348,11 @@
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="3"/>
-      <c r="J38" s="111" t="s">
+      <c r="J38" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="111"/>
-      <c r="L38" s="112"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="114"/>
       <c r="M38" s="92"/>
       <c r="N38" s="94"/>
       <c r="O38" s="17" t="s">
@@ -4363,7 +4465,7 @@
         <v>1750</v>
       </c>
       <c r="P45" s="86"/>
-      <c r="R45" s="116">
+      <c r="R45" s="111">
         <f>K35+O40+F33</f>
         <v>66892.5</v>
       </c>
@@ -4377,7 +4479,7 @@
       <c r="J47" t="s">
         <v>29</v>
       </c>
-      <c r="R47" s="116">
+      <c r="R47" s="111">
         <f>S34+O40+F33</f>
         <v>49817.5</v>
       </c>
@@ -4409,11 +4511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5196,11 +5298,21 @@
       <c r="B21" s="78">
         <v>2</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
+      <c r="C21" s="104">
+        <v>162.5</v>
+      </c>
+      <c r="D21" s="77">
+        <v>187.5</v>
+      </c>
+      <c r="E21" s="104">
+        <v>187.5</v>
+      </c>
+      <c r="F21" s="104">
+        <v>193.75</v>
+      </c>
+      <c r="G21" s="104">
+        <v>112.5</v>
+      </c>
       <c r="H21" s="104">
         <v>50</v>
       </c>
@@ -5213,10 +5325,12 @@
       <c r="K21" s="104">
         <v>175</v>
       </c>
-      <c r="L21" s="104"/>
+      <c r="L21" s="104">
+        <v>175</v>
+      </c>
       <c r="M21" s="13">
         <f t="shared" si="0"/>
-        <v>562.5</v>
+        <v>1581.25</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -5401,23 +5515,23 @@
       </c>
       <c r="C31" s="12">
         <f>SUM(C3:C29)</f>
-        <v>1837.5</v>
+        <v>2000</v>
       </c>
       <c r="D31" s="12">
         <f>SUM(D3:D29)</f>
-        <v>2175</v>
+        <v>2362.5</v>
       </c>
       <c r="E31" s="12">
         <f>SUM(E3:E29)</f>
-        <v>1525</v>
+        <v>1712.5</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" ref="F31:M31" si="1">SUM(F3:F29)</f>
-        <v>2515</v>
+        <v>2708.75</v>
       </c>
       <c r="G31" s="12">
         <f t="shared" si="1"/>
-        <v>1162.5</v>
+        <v>1275</v>
       </c>
       <c r="H31" s="12">
         <f t="shared" si="1"/>
@@ -5437,11 +5551,11 @@
       </c>
       <c r="L31" s="12">
         <f t="shared" si="1"/>
-        <v>2531.25</v>
+        <v>2706.25</v>
       </c>
       <c r="M31" s="107">
         <f t="shared" si="1"/>
-        <v>18683.75</v>
+        <v>19702.5</v>
       </c>
     </row>
     <row r="37" spans="3:13">
@@ -5449,17 +5563,21 @@
         <f>SUM(C14:L18)</f>
         <v>4799.75</v>
       </c>
+      <c r="I37" s="110">
+        <f>SUM('Buisness Projection'!U6:U20)-SUM('Buisness Projection'!T6:T20)</f>
+        <v>2276.25</v>
+      </c>
       <c r="M37" s="12">
         <f>SUM(M14:M18)</f>
         <v>4799.75</v>
       </c>
     </row>
     <row r="38" spans="3:13">
-      <c r="C38" s="12">
+      <c r="C38" s="117">
         <f>((C37/12.5)/10)/5</f>
         <v>7.6796000000000006</v>
       </c>
-      <c r="M38" s="115">
+      <c r="M38" s="110">
         <f>SUM('Buisness Projection'!T16:T20)</f>
         <v>3750</v>
       </c>
@@ -5472,6 +5590,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>